<commit_message>
test and framework done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\Re-Usable Edited Framwork\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\RE-Framework Common Template v0.03\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771EAE19-E7EA-40BE-A12C-0E326E4DA103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7401A5FD-F218-4ADF-A97F-6A1377F52873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>dthilakarathne@innobothealth.com,dthilakarathne@innobothealth.com</t>
+  </si>
+  <si>
+    <t>webPageURL</t>
+  </si>
+  <si>
+    <t>https://www.rpasamples.com/suppliers</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,7 +278,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,9 +296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -331,7 +336,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -437,7 +442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -579,7 +584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,7 +595,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -713,7 +718,7 @@
       <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -735,7 +740,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
create log template modified
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\RE-Framework Common Template v0.03\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7401A5FD-F218-4ADF-A97F-6A1377F52873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8559B8E7-8682-41C2-94EC-DED51CC83AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>https://www.rpasamples.com/suppliers</t>
+  </si>
+  <si>
+    <t>Write_LogPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Dinuka Thilakarathne\OneDrive\Documents\UiPath\RE-Framework Common Template v0.03\Data\Output\</t>
   </si>
 </sst>
 </file>
@@ -595,7 +601,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -748,7 +754,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>